<commit_message>
update grades for midterm 1
</commit_message>
<xml_diff>
--- a/grades/grades.xlsx
+++ b/grades/grades.xlsx
@@ -466,10 +466,10 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -481,7 +481,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -495,7 +495,7 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -509,6 +509,10 @@
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F3" s="0" t="n">
+        <f aca="false">51/60</f>
+        <v>0.85</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -531,6 +535,10 @@
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">61/60</f>
+        <v>1.01666666666667</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -542,6 +550,10 @@
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="F6" s="0" t="n">
+        <f aca="false">51/60</f>
+        <v>0.85</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -564,7 +576,7 @@
       <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <f aca="false">57/60</f>
         <v>0.95</v>
       </c>
@@ -579,6 +591,10 @@
       <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="F9" s="0" t="n">
+        <f aca="false">40/60</f>
+        <v>0.666666666666667</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -590,7 +606,7 @@
       <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <f aca="false">55/60</f>
         <v>0.916666666666667</v>
       </c>
@@ -638,6 +654,10 @@
       <c r="C14" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="F14" s="0" t="n">
+        <f aca="false">41/60</f>
+        <v>0.683333333333333</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -693,7 +713,7 @@
       <c r="C19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <f aca="false">50/60</f>
         <v>0.833333333333333</v>
       </c>
@@ -719,7 +739,7 @@
       <c r="C21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <f aca="false">50/60</f>
         <v>0.833333333333333</v>
       </c>
@@ -734,7 +754,7 @@
       <c r="C22" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="1" t="n">
         <f aca="false">54/60</f>
         <v>0.9</v>
       </c>
@@ -749,7 +769,7 @@
       <c r="C23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="1" t="n">
         <f aca="false">57/60</f>
         <v>0.95</v>
       </c>
@@ -797,7 +817,7 @@
       <c r="C27" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="1" t="n">
         <f aca="false">57/60</f>
         <v>0.95</v>
       </c>
@@ -812,6 +832,10 @@
       <c r="C28" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="F28" s="0" t="n">
+        <f aca="false">58/60</f>
+        <v>0.966666666666667</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
@@ -834,7 +858,7 @@
       <c r="C30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="1" t="n">
         <f aca="false">52/60</f>
         <v>0.866666666666667</v>
       </c>
@@ -860,6 +884,10 @@
       <c r="C32" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="F32" s="0" t="n">
+        <f aca="false">42/60</f>
+        <v>0.7</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -871,7 +899,7 @@
       <c r="C33" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33" s="1" t="n">
         <f aca="false">48/60</f>
         <v>0.8</v>
       </c>
@@ -897,6 +925,10 @@
       <c r="C35" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="F35" s="0" t="n">
+        <f aca="false">40/60</f>
+        <v>0.666666666666667</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
@@ -919,7 +951,7 @@
       <c r="C37" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F37" s="1" t="n">
         <f aca="false">53/60</f>
         <v>0.883333333333333</v>
       </c>

</xml_diff>

<commit_message>
midterm 1 grade update
</commit_message>
<xml_diff>
--- a/grades/grades.xlsx
+++ b/grades/grades.xlsx
@@ -368,8 +368,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -437,12 +438,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -466,10 +471,10 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -509,7 +514,7 @@
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
         <f aca="false">51/60</f>
         <v>0.85</v>
       </c>
@@ -524,6 +529,10 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F4" s="0" t="n">
+        <f aca="false">40/60</f>
+        <v>0.666666666666667</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -535,7 +544,7 @@
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="2" t="n">
         <f aca="false">61/60</f>
         <v>1.01666666666667</v>
       </c>
@@ -550,7 +559,7 @@
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="2" t="n">
         <f aca="false">51/60</f>
         <v>0.85</v>
       </c>
@@ -591,7 +600,7 @@
       <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="2" t="n">
         <f aca="false">40/60</f>
         <v>0.666666666666667</v>
       </c>
@@ -621,6 +630,10 @@
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="F11" s="0" t="n">
+        <f aca="false">55/60</f>
+        <v>0.916666666666667</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -632,6 +645,10 @@
       <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="F12" s="0" t="n">
+        <f aca="false">54/60</f>
+        <v>0.9</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -643,6 +660,10 @@
       <c r="C13" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="F13" s="0" t="n">
+        <f aca="false">52/60</f>
+        <v>0.866666666666667</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -654,12 +675,12 @@
       <c r="C14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="2" t="n">
         <f aca="false">41/60</f>
         <v>0.683333333333333</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -668,6 +689,10 @@
       </c>
       <c r="C15" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <f aca="false">50/60</f>
+        <v>0.833333333333333</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -728,6 +753,10 @@
       <c r="C20" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="F20" s="0" t="n">
+        <f aca="false">(60-14)/60</f>
+        <v>0.766666666666667</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -795,6 +824,10 @@
       <c r="C25" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="F25" s="0" t="n">
+        <f aca="false">51/60</f>
+        <v>0.85</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
@@ -832,7 +865,7 @@
       <c r="C28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28" s="2" t="n">
         <f aca="false">58/60</f>
         <v>0.966666666666667</v>
       </c>
@@ -884,7 +917,7 @@
       <c r="C32" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32" s="2" t="n">
         <f aca="false">42/60</f>
         <v>0.7</v>
       </c>
@@ -914,6 +947,10 @@
       <c r="C34" s="1" t="s">
         <v>101</v>
       </c>
+      <c r="F34" s="0" t="n">
+        <f aca="false">40/60</f>
+        <v>0.666666666666667</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
@@ -925,7 +962,7 @@
       <c r="C35" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="F35" s="2" t="n">
         <f aca="false">40/60</f>
         <v>0.666666666666667</v>
       </c>

</xml_diff>

<commit_message>
grade update, and storing essays
</commit_message>
<xml_diff>
--- a/grades/grades.xlsx
+++ b/grades/grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Midterm 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Paper</t>
   </si>
   <si>
     <t xml:space="preserve">Jordan</t>
@@ -438,12 +441,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -468,13 +475,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.58"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -489,16 +499,19 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>1</v>
@@ -506,13 +519,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="n">
         <f aca="false">51/60</f>
@@ -521,28 +534,28 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="n">
         <f aca="false">40/60</f>
         <v>0.666666666666667</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2" t="n">
         <f aca="false">61/60</f>
@@ -551,13 +564,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="n">
         <f aca="false">51/60</f>
@@ -566,24 +579,24 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F8" s="1" t="n">
         <f aca="false">57/60</f>
@@ -592,13 +605,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9" s="2" t="n">
         <f aca="false">40/60</f>
@@ -607,13 +620,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F10" s="1" t="n">
         <f aca="false">55/60</f>
@@ -622,121 +635,129 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="F11" s="3" t="n">
         <f aca="false">55/60</f>
         <v>0.916666666666667</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="F12" s="3" t="n">
         <f aca="false">54/60</f>
         <v>0.9</v>
       </c>
+      <c r="G12" s="0" t="n">
+        <f aca="false">75/100</f>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="F13" s="3" t="n">
         <f aca="false">52/60</f>
         <v>0.866666666666667</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F14" s="2" t="n">
         <f aca="false">41/60</f>
         <v>0.683333333333333</v>
       </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">90/100</f>
+        <v>0.9</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="F15" s="3" t="n">
         <f aca="false">50/60</f>
         <v>0.833333333333333</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">50/60</f>
@@ -745,28 +766,28 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="F20" s="3" t="n">
         <f aca="false">(60-14)/60</f>
         <v>0.766666666666667</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F21" s="1" t="n">
         <f aca="false">50/60</f>
@@ -775,13 +796,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F22" s="1" t="n">
         <f aca="false">54/60</f>
@@ -790,13 +811,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F23" s="1" t="n">
         <f aca="false">57/60</f>
@@ -805,65 +826,69 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F25" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="F25" s="3" t="n">
         <f aca="false">51/60</f>
         <v>0.85</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F27" s="1" t="n">
         <f aca="false">57/60</f>
         <v>0.95</v>
       </c>
+      <c r="G27" s="0" t="n">
+        <f aca="false">95/100</f>
+        <v>0.95</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F28" s="2" t="n">
         <f aca="false">58/60</f>
@@ -872,24 +897,24 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F30" s="1" t="n">
         <f aca="false">52/60</f>
@@ -898,24 +923,24 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F32" s="2" t="n">
         <f aca="false">42/60</f>
@@ -924,13 +949,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F33" s="1" t="n">
         <f aca="false">48/60</f>
@@ -939,28 +964,28 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F34" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="F34" s="3" t="n">
         <f aca="false">40/60</f>
         <v>0.666666666666667</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F35" s="2" t="n">
         <f aca="false">40/60</f>
@@ -969,24 +994,24 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F37" s="1" t="n">
         <f aca="false">53/60</f>
@@ -995,13 +1020,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added midterm 2 and a grade update.
</commit_message>
<xml_diff>
--- a/grades/grades.xlsx
+++ b/grades/grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -37,13 +37,7 @@
     <t xml:space="preserve">Final Paper</t>
   </si>
   <si>
-    <t xml:space="preserve">Jordan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hanson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jhanson2@whittier.edu</t>
+    <t xml:space="preserve">Final Project</t>
   </si>
   <si>
     <t xml:space="preserve">Lucy</t>
@@ -82,15 +76,6 @@
     <t xml:space="preserve">lcastil1@poets.whittier.edu</t>
   </si>
   <si>
-    <t xml:space="preserve">Jude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pazier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jpazier@poets.whittier.edu</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cyrus</t>
   </si>
   <si>
@@ -235,15 +220,6 @@
     <t xml:space="preserve">ahennes1@poets.whittier.edu</t>
   </si>
   <si>
-    <t xml:space="preserve">Skye</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mendoza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">amendoz7@poets.whittier.edu</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nohely</t>
   </si>
   <si>
@@ -280,15 +256,6 @@
     <t xml:space="preserve">lfrates@poets.whittier.edu</t>
   </si>
   <si>
-    <t xml:space="preserve">Nolan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nmorton@poets.whittier.edu</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jamie</t>
   </si>
   <si>
@@ -298,15 +265,6 @@
     <t xml:space="preserve">jluna3@poets.whittier.edu</t>
   </si>
   <si>
-    <t xml:space="preserve">Madi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gasca Reyes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mgascare@poets.whittier.edu</t>
-  </si>
-  <si>
     <t xml:space="preserve">Johnathon</t>
   </si>
   <si>
@@ -338,15 +296,6 @@
   </si>
   <si>
     <t xml:space="preserve">kpham2@poets.whittier.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alberto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juan Y Seva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ajuanyse@poets.whittier.edu</t>
   </si>
   <si>
     <t xml:space="preserve">Emilia</t>
@@ -441,16 +390,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -475,15 +420,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -502,397 +448,473 @@
       <c r="G1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <f aca="false">51/60</f>
+        <v>0.85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2" t="n">
+        <f aca="false">40/60</f>
+        <v>0.666666666666667</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <f aca="false">61/60</f>
+        <v>1.01666666666667</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <f aca="false">51/60</f>
         <v>0.85</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="n">
+      <c r="H5" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <f aca="false">57/60</f>
+        <v>0.95</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">95/100</f>
+        <v>0.95</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2" t="n">
         <f aca="false">40/60</f>
         <v>0.666666666666667</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <f aca="false">61/60</f>
-        <v>1.01666666666667</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <f aca="false">51/60</f>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
+      <c r="H7" s="0" t="n">
+        <f aca="false">5/10</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="n">
-        <f aca="false">57/60</f>
-        <v>0.95</v>
+        <f aca="false">55/60</f>
+        <v>0.916666666666667</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F9" s="2" t="n">
-        <f aca="false">40/60</f>
-        <v>0.666666666666667</v>
+        <f aca="false">55/60</f>
+        <v>0.916666666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <f aca="false">55/60</f>
-        <v>0.916666666666667</v>
+        <v>32</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <f aca="false">54/60</f>
+        <v>0.9</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">75/100</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="3" t="n">
-        <f aca="false">55/60</f>
-        <v>0.916666666666667</v>
+        <v>35</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <f aca="false">52/60</f>
+        <v>0.866666666666667</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="3" t="n">
-        <f aca="false">54/60</f>
+        <v>38</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <f aca="false">41/60</f>
+        <v>0.683333333333333</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <f aca="false">90/100</f>
         <v>0.9</v>
       </c>
-      <c r="G12" s="0" t="n">
-        <f aca="false">75/100</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="3" t="n">
-        <f aca="false">52/60</f>
-        <v>0.866666666666667</v>
+        <v>41</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <f aca="false">50/60</f>
+        <v>0.833333333333333</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="2" t="n">
-        <f aca="false">41/60</f>
-        <v>0.683333333333333</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <f aca="false">90/100</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="3" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="1" t="n">
         <f aca="false">50/60</f>
         <v>0.833333333333333</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>52</v>
+      <c r="H17" s="0" t="n">
+        <f aca="false">9/10</f>
+        <v>0.9</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <f aca="false">(60-14)/60</f>
+        <v>0.766666666666667</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">50/60</f>
         <v>0.833333333333333</v>
       </c>
+      <c r="H19" s="0" t="n">
+        <f aca="false">9/10</f>
+        <v>0.9</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="3" t="n">
-        <f aca="false">(60-14)/60</f>
-        <v>0.766666666666667</v>
+        <v>62</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <f aca="false">54/60</f>
+        <v>0.9</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F21" s="1" t="n">
-        <f aca="false">50/60</f>
-        <v>0.833333333333333</v>
+        <f aca="false">57/60</f>
+        <v>0.95</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="1" t="n">
-        <f aca="false">54/60</f>
+        <v>68</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <f aca="false">51/60</f>
+        <v>0.85</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <f aca="false">9/10</f>
         <v>0.9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" s="1" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="1" t="n">
         <f aca="false">57/60</f>
         <v>0.95</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>73</v>
+      <c r="G24" s="0" t="n">
+        <f aca="false">95/100</f>
+        <v>0.95</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="3" t="n">
-        <f aca="false">51/60</f>
-        <v>0.85</v>
+        <v>77</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <f aca="false">58/60</f>
+        <v>0.966666666666667</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <f aca="false">52/60</f>
+        <v>0.866666666666667</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F27" s="1" t="n">
-        <f aca="false">57/60</f>
-        <v>0.95</v>
-      </c>
-      <c r="G27" s="0" t="n">
-        <f aca="false">95/100</f>
-        <v>0.95</v>
+        <v>83</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <f aca="false">42/60</f>
+        <v>0.7</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <f aca="false">9/10</f>
+        <v>0.9</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F28" s="2" t="n">
-        <f aca="false">58/60</f>
-        <v>0.966666666666667</v>
+      <c r="F28" s="1" t="n">
+        <f aca="false">48/60</f>
+        <v>0.8</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,6 +927,10 @@
       <c r="C29" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="F29" s="2" t="n">
+        <f aca="false">40/60</f>
+        <v>0.666666666666667</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
@@ -916,9 +942,9 @@
       <c r="C30" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F30" s="1" t="n">
-        <f aca="false">52/60</f>
-        <v>0.866666666666667</v>
+      <c r="F30" s="2" t="n">
+        <f aca="false">40/60</f>
+        <v>0.666666666666667</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -931,6 +957,14 @@
       <c r="C31" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="F31" s="1" t="n">
+        <f aca="false">53/60</f>
+        <v>0.883333333333333</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
@@ -941,92 +975,6 @@
       </c>
       <c r="C32" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="F32" s="2" t="n">
-        <f aca="false">42/60</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F33" s="1" t="n">
-        <f aca="false">48/60</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F34" s="3" t="n">
-        <f aca="false">40/60</f>
-        <v>0.666666666666667</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F35" s="2" t="n">
-        <f aca="false">40/60</f>
-        <v>0.666666666666667</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F37" s="1" t="n">
-        <f aca="false">53/60</f>
-        <v>0.883333333333333</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
big grade update, new essays
</commit_message>
<xml_diff>
--- a/grades/grades.xlsx
+++ b/grades/grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -148,15 +148,6 @@
     <t xml:space="preserve">obutler@poets.whittier.edu</t>
   </si>
   <si>
-    <t xml:space="preserve">Gia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gprado2@poets.whittier.edu</t>
-  </si>
-  <si>
     <t xml:space="preserve">William</t>
   </si>
   <si>
@@ -227,15 +218,6 @@
   </si>
   <si>
     <t xml:space="preserve">nlopez7@poets.whittier.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emmanuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cevallos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ecevallo@poets.whittier.edu</t>
   </si>
   <si>
     <t xml:space="preserve">Chianti</t>
@@ -420,13 +402,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.59"/>
@@ -466,6 +448,10 @@
         <f aca="false">51/60</f>
         <v>0.85</v>
       </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">85/100</f>
+        <v>0.85</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -481,6 +467,10 @@
         <f aca="false">40/60</f>
         <v>0.666666666666667</v>
       </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">85/100</f>
+        <v>0.85</v>
+      </c>
       <c r="H3" s="0" t="n">
         <f aca="false">10/10</f>
         <v>1</v>
@@ -561,6 +551,10 @@
         <f aca="false">40/60</f>
         <v>0.666666666666667</v>
       </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">80/100</f>
+        <v>0.8</v>
+      </c>
       <c r="H7" s="0" t="n">
         <f aca="false">5/10</f>
         <v>0.5</v>
@@ -580,6 +574,10 @@
         <f aca="false">55/60</f>
         <v>0.916666666666667</v>
       </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">90/100</f>
+        <v>0.9</v>
+      </c>
       <c r="H8" s="0" t="n">
         <f aca="false">10/10</f>
         <v>1</v>
@@ -599,6 +597,10 @@
         <f aca="false">55/60</f>
         <v>0.916666666666667</v>
       </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">90/100</f>
+        <v>0.9</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -633,6 +635,14 @@
         <f aca="false">52/60</f>
         <v>0.866666666666667</v>
       </c>
+      <c r="G11" s="0" t="n">
+        <f aca="false">75/100</f>
+        <v>0.75</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -667,6 +677,10 @@
         <f aca="false">50/60</f>
         <v>0.833333333333333</v>
       </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">95/100</f>
+        <v>0.95</v>
+      </c>
       <c r="H13" s="0" t="n">
         <f aca="false">10/10</f>
         <v>1</v>
@@ -704,6 +718,14 @@
       <c r="C16" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="F16" s="1" t="n">
+        <f aca="false">50/60</f>
+        <v>0.833333333333333</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <f aca="false">9/10</f>
+        <v>0.9</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -715,13 +737,17 @@
       <c r="C17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="1" t="n">
-        <f aca="false">50/60</f>
-        <v>0.833333333333333</v>
+      <c r="F17" s="2" t="n">
+        <f aca="false">(60-14)/60</f>
+        <v>0.766666666666667</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">60/100</f>
+        <v>0.6</v>
       </c>
       <c r="H17" s="0" t="n">
-        <f aca="false">9/10</f>
-        <v>0.9</v>
+        <f aca="false">10/10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -734,13 +760,13 @@
       <c r="C18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="2" t="n">
-        <f aca="false">(60-14)/60</f>
-        <v>0.766666666666667</v>
+      <c r="F18" s="1" t="n">
+        <f aca="false">50/60</f>
+        <v>0.833333333333333</v>
       </c>
       <c r="H18" s="0" t="n">
-        <f aca="false">10/10</f>
-        <v>1</v>
+        <f aca="false">9/10</f>
+        <v>0.9</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,12 +780,16 @@
         <v>59</v>
       </c>
       <c r="F19" s="1" t="n">
-        <f aca="false">50/60</f>
-        <v>0.833333333333333</v>
+        <f aca="false">54/60</f>
+        <v>0.9</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <f aca="false">95/100</f>
+        <v>0.95</v>
       </c>
       <c r="H19" s="0" t="n">
-        <f aca="false">9/10</f>
-        <v>0.9</v>
+        <f aca="false">10/10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,12 +803,8 @@
         <v>62</v>
       </c>
       <c r="F20" s="1" t="n">
-        <f aca="false">54/60</f>
-        <v>0.9</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <f aca="false">10/10</f>
-        <v>1</v>
+        <f aca="false">57/60</f>
+        <v>0.95</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,9 +817,17 @@
       <c r="C21" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="1" t="n">
-        <f aca="false">57/60</f>
-        <v>0.95</v>
+      <c r="F21" s="2" t="n">
+        <f aca="false">51/60</f>
+        <v>0.85</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">90/100</f>
+        <v>0.9</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <f aca="false">9/10</f>
+        <v>0.9</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -806,13 +840,17 @@
       <c r="C22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="2" t="n">
-        <f aca="false">51/60</f>
-        <v>0.85</v>
+      <c r="F22" s="1" t="n">
+        <f aca="false">57/60</f>
+        <v>0.95</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <f aca="false">95/100</f>
+        <v>0.95</v>
       </c>
       <c r="H22" s="0" t="n">
-        <f aca="false">9/10</f>
-        <v>0.9</v>
+        <f aca="false">10/10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -825,6 +863,14 @@
       <c r="C23" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="F23" s="2" t="n">
+        <f aca="false">58/60</f>
+        <v>0.966666666666667</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <f aca="false">100/100</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
@@ -837,16 +883,8 @@
         <v>74</v>
       </c>
       <c r="F24" s="1" t="n">
-        <f aca="false">57/60</f>
-        <v>0.95</v>
-      </c>
-      <c r="G24" s="0" t="n">
-        <f aca="false">95/100</f>
-        <v>0.95</v>
-      </c>
-      <c r="H24" s="0" t="n">
-        <f aca="false">10/10</f>
-        <v>1</v>
+        <f aca="false">52/60</f>
+        <v>0.866666666666667</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -860,8 +898,16 @@
         <v>77</v>
       </c>
       <c r="F25" s="2" t="n">
-        <f aca="false">58/60</f>
-        <v>0.966666666666667</v>
+        <f aca="false">42/60</f>
+        <v>0.7</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <f aca="false">95/100</f>
+        <v>0.95</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <f aca="false">9/10</f>
+        <v>0.9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,52 +915,52 @@
         <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="F26" s="1" t="n">
-        <f aca="false">52/60</f>
-        <v>0.866666666666667</v>
+        <f aca="false">48/60</f>
+        <v>0.8</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">90/100</f>
+        <v>0.9</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="F27" s="2" t="n">
-        <f aca="false">42/60</f>
-        <v>0.7</v>
-      </c>
-      <c r="H27" s="0" t="n">
-        <f aca="false">9/10</f>
-        <v>0.9</v>
+        <f aca="false">40/60</f>
+        <v>0.666666666666667</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F28" s="1" t="n">
-        <f aca="false">48/60</f>
-        <v>0.8</v>
-      </c>
-      <c r="H28" s="0" t="n">
-        <f aca="false">10/10</f>
-        <v>1</v>
+      <c r="F28" s="2" t="n">
+        <f aca="false">40/60</f>
+        <v>0.666666666666667</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -927,9 +973,13 @@
       <c r="C29" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F29" s="2" t="n">
-        <f aca="false">40/60</f>
-        <v>0.666666666666667</v>
+      <c r="F29" s="1" t="n">
+        <f aca="false">53/60</f>
+        <v>0.883333333333333</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,40 +991,6 @@
       </c>
       <c r="C30" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F30" s="2" t="n">
-        <f aca="false">40/60</f>
-        <v>0.666666666666667</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F31" s="1" t="n">
-        <f aca="false">53/60</f>
-        <v>0.883333333333333</v>
-      </c>
-      <c r="H31" s="0" t="n">
-        <f aca="false">10/10</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last grade update with midterm 2
</commit_message>
<xml_diff>
--- a/grades/grades.xlsx
+++ b/grades/grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="97">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -40,6 +40,21 @@
     <t xml:space="preserve">Final Project</t>
   </si>
   <si>
+    <t xml:space="preserve">Midterm 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In-class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw Scores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w/ Curve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Letter</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lucy</t>
   </si>
   <si>
@@ -49,6 +64,9 @@
     <t xml:space="preserve">lcampbel@poets.whittier.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nate</t>
   </si>
   <si>
@@ -58,6 +76,9 @@
     <t xml:space="preserve">nmedina1@poets.whittier.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">A-</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kamarina</t>
   </si>
   <si>
@@ -94,6 +115,9 @@
     <t xml:space="preserve">kumeda@poets.whittier.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">C+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Annalise</t>
   </si>
   <si>
@@ -121,6 +145,9 @@
     <t xml:space="preserve">pahire@poets.whittier.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tyler</t>
   </si>
   <si>
@@ -175,6 +202,9 @@
     <t xml:space="preserve">rlawrenc@poets.whittier.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">B+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Filipp</t>
   </si>
   <si>
@@ -260,6 +290,9 @@
   </si>
   <si>
     <t xml:space="preserve">sgarrido@poets.whittier.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-</t>
   </si>
   <si>
     <t xml:space="preserve">Kayla</t>
@@ -384,16 +417,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M29" activeCellId="0" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,16 +451,31 @@
       <c r="H1" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="n">
         <f aca="false">51/60</f>
@@ -434,16 +485,39 @@
         <f aca="false">85/100</f>
         <v>0.85</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <f aca="false">45/50</f>
+        <v>0.9</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <f aca="false">0.2*F2+0.2*G2+0.2*H2+0.2*I2+0.2*J2</f>
+        <v>0.92</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <f aca="false">K2+0.03</f>
+        <v>0.95</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F3" s="2" t="n">
         <f aca="false">40/60</f>
@@ -457,16 +531,35 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="0" t="n">
+        <f aca="false">44/50</f>
+        <v>0.88</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <f aca="false">0.2*F3+0.2*G3+0.2*H3+0.2*I3+0.2*J3</f>
+        <v>0.879333333333334</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <f aca="false">K3+0.03</f>
+        <v>0.909333333333334</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F4" s="2" t="n">
         <f aca="false">61/60</f>
@@ -480,16 +573,35 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I4" s="0" t="n">
+        <f aca="false">48/50</f>
+        <v>0.96</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <f aca="false">0.2*F4+0.2*G4+0.2*H4+0.2*I4+0.2*J4</f>
+        <v>0.995333333333334</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <f aca="false">K4+0.03</f>
+        <v>1.02533333333333</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F5" s="2" t="n">
         <f aca="false">51/60</f>
@@ -503,16 +615,35 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I5" s="0" t="n">
+        <f aca="false">47.5/50</f>
+        <v>0.95</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <f aca="false">0.2*F5+0.2*G5+0.2*H5+0.2*I5+0.2*J5</f>
+        <v>0.96</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <f aca="false">K5+0.03</f>
+        <v>0.99</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="n">
         <f aca="false">57/60</f>
@@ -526,16 +657,35 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I6" s="0" t="n">
+        <f aca="false">45/50</f>
+        <v>0.9</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">0.2*F6+0.2*G6+0.2*H6+0.2*I6+0.2*J6</f>
+        <v>0.96</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <f aca="false">K6+0.03</f>
+        <v>0.99</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F7" s="2" t="n">
         <f aca="false">40/60</f>
@@ -549,16 +699,35 @@
         <f aca="false">5/10</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I7" s="0" t="n">
+        <f aca="false">33/50</f>
+        <v>0.66</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <f aca="false">0.2*F7+0.2*G7+0.2*H7+0.2*I7+0.2*J7</f>
+        <v>0.725333333333333</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <f aca="false">K7+0.03</f>
+        <v>0.755333333333333</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="n">
         <f aca="false">55/60</f>
@@ -572,16 +741,35 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I8" s="0" t="n">
+        <f aca="false">47.5/50</f>
+        <v>0.95</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">0.2*F8+0.2*G8+0.2*H8+0.2*I8+0.2*J8</f>
+        <v>0.953333333333333</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <f aca="false">K8+0.03</f>
+        <v>0.983333333333333</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F9" s="2" t="n">
         <f aca="false">55/60</f>
@@ -591,16 +779,39 @@
         <f aca="false">90/100</f>
         <v>0.9</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <f aca="false">47/50</f>
+        <v>0.94</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <f aca="false">0.2*F9+0.2*G9+0.2*H9+0.2*I9+0.2*J9</f>
+        <v>0.951333333333333</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <f aca="false">K9+0.03</f>
+        <v>0.981333333333333</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F10" s="2" t="n">
         <f aca="false">54/60</f>
@@ -610,16 +821,39 @@
         <f aca="false">75/100</f>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <f aca="false">44/50</f>
+        <v>0.88</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <f aca="false">0.2*F10+0.2*G10+0.2*H10+0.2*I10+0.2*J10</f>
+        <v>0.706</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <f aca="false">K10+0.03</f>
+        <v>0.736</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F11" s="2" t="n">
         <f aca="false">52/60</f>
@@ -633,16 +867,35 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I11" s="0" t="n">
+        <f aca="false">47.5/50</f>
+        <v>0.95</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <f aca="false">0.2*F11+0.2*G11+0.2*H11+0.2*I11+0.2*J11</f>
+        <v>0.913333333333333</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <f aca="false">K11+0.03</f>
+        <v>0.943333333333333</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F12" s="2" t="n">
         <f aca="false">41/60</f>
@@ -652,16 +905,36 @@
         <f aca="false">90/100</f>
         <v>0.9</v>
       </c>
+      <c r="H12" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <f aca="false">0/50</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <f aca="false">0.2*F12+0.2*G12+0.2*H12+0.2*I12+0.2*J12</f>
+        <v>0.516666666666667</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <f aca="false">K12+0.03</f>
+        <v>0.546666666666667</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F13" s="2" t="n">
         <f aca="false">50/60</f>
@@ -675,31 +948,70 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I13" s="0" t="n">
+        <f aca="false">47/50</f>
+        <v>0.94</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <f aca="false">0.2*F13+0.2*G13+0.2*H13+0.2*I13+0.2*J13</f>
+        <v>0.944666666666667</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <f aca="false">K13+0.03</f>
+        <v>0.974666666666666</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">80/100</f>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H14" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <f aca="false">42/50</f>
+        <v>0.84</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <f aca="false">0.2*F14+0.2*G14+0.2*H14+0.2*I14+0.2*J14</f>
+        <v>0.528</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <f aca="false">K14+0.03</f>
+        <v>0.558</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">50/60</f>
@@ -713,16 +1025,35 @@
         <f aca="false">9/10</f>
         <v>0.9</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I15" s="0" t="n">
+        <f aca="false">45.5/50</f>
+        <v>0.91</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <f aca="false">0.2*F15+0.2*G15+0.2*H15+0.2*I15+0.2*J15</f>
+        <v>0.908666666666667</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <f aca="false">K15+0.03</f>
+        <v>0.938666666666667</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F16" s="2" t="n">
         <f aca="false">(60-14)/60</f>
@@ -736,35 +1067,77 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I16" s="0" t="n">
+        <f aca="false">41/50</f>
+        <v>0.82</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <f aca="false">0.2*F16+0.2*G16+0.2*H16+0.2*I16+0.2*J16</f>
+        <v>0.837333333333334</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <f aca="false">K16+0.03</f>
+        <v>0.867333333333333</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">50/60</f>
         <v>0.833333333333333</v>
       </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">100/100</f>
+        <v>1</v>
+      </c>
       <c r="H17" s="0" t="n">
         <f aca="false">9/10</f>
         <v>0.9</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I17" s="0" t="n">
+        <f aca="false">42.5/50</f>
+        <v>0.85</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <f aca="false">0.2*F17+0.2*G17+0.2*H17+0.2*I17+0.2*J17</f>
+        <v>0.916666666666667</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <f aca="false">K17+0.03</f>
+        <v>0.946666666666667</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">54/60</f>
@@ -778,16 +1151,35 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I18" s="0" t="n">
+        <f aca="false">47/50</f>
+        <v>0.94</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <f aca="false">0.2*F18+0.2*G18+0.2*H18+0.2*I18+0.2*J18</f>
+        <v>0.958</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <f aca="false">K18+0.03</f>
+        <v>0.988</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">57/60</f>
@@ -797,16 +1189,39 @@
         <f aca="false">95/100</f>
         <v>0.95</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H19" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <f aca="false">47/50</f>
+        <v>0.94</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <f aca="false">0.2*F19+0.2*G19+0.2*H19+0.2*I19+0.2*J19</f>
+        <v>0.968</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <f aca="false">K19+0.03</f>
+        <v>0.998</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="F20" s="2" t="n">
         <f aca="false">51/60</f>
@@ -820,16 +1235,35 @@
         <f aca="false">9/10</f>
         <v>0.9</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I20" s="0" t="n">
+        <f aca="false">42/50</f>
+        <v>0.84</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <f aca="false">0.2*F20+0.2*G20+0.2*H20+0.2*I20+0.2*J20</f>
+        <v>0.898</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <f aca="false">K20+0.03</f>
+        <v>0.928</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="F21" s="1" t="n">
         <f aca="false">57/60</f>
@@ -843,16 +1277,35 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I21" s="0" t="n">
+        <f aca="false">49/50</f>
+        <v>0.98</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <f aca="false">0.2*F21+0.2*G21+0.2*H21+0.2*I21+0.2*J21</f>
+        <v>0.976</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <f aca="false">K21+0.03</f>
+        <v>1.006</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="F22" s="2" t="n">
         <f aca="false">58/60</f>
@@ -862,35 +1315,81 @@
         <f aca="false">100/100</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H22" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <f aca="false">50/50</f>
+        <v>1</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <f aca="false">0.2*F22+0.2*G22+0.2*H22+0.2*I22+0.2*J22</f>
+        <v>0.993333333333333</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <f aca="false">K22+0.03</f>
+        <v>1.02333333333333</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F23" s="1" t="n">
         <f aca="false">52/60</f>
         <v>0.866666666666667</v>
       </c>
       <c r="G23" s="0" t="n">
-        <f aca="false">50/100</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">80/100</f>
+        <v>0.8</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <f aca="false">85/100</f>
+        <v>0.85</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <f aca="false">48/50</f>
+        <v>0.96</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <f aca="false">0.2*F23+0.2*G23+0.2*H23+0.2*I23+0.2*J23</f>
+        <v>0.895333333333334</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <f aca="false">K23+0.03</f>
+        <v>0.925333333333334</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F24" s="2" t="n">
         <f aca="false">42/60</f>
@@ -904,16 +1403,35 @@
         <f aca="false">9/10</f>
         <v>0.9</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I24" s="0" t="n">
+        <f aca="false">0/50</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <f aca="false">0.2*F24+0.2*G24+0.2*H24+0.2*I24+0.2*J24</f>
+        <v>0.71</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <f aca="false">K24+0.03</f>
+        <v>0.74</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F25" s="1" t="n">
         <f aca="false">48/60</f>
@@ -927,31 +1445,77 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I25" s="0" t="n">
+        <f aca="false">46/50</f>
+        <v>0.92</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <f aca="false">0.2*F25+0.2*G25+0.2*H25+0.2*I25+0.2*J25</f>
+        <v>0.924</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <f aca="false">K25+0.03</f>
+        <v>0.954</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="F26" s="2" t="n">
         <f aca="false">40/60</f>
         <v>0.666666666666667</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="0" t="n">
+        <f aca="false">90/100</f>
+        <v>0.9</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <f aca="false">43/50</f>
+        <v>0.86</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <f aca="false">0.2*F26+0.2*G26+0.2*H26+0.2*I26+0.2*J26</f>
+        <v>0.685333333333333</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <f aca="false">K26+0.03</f>
+        <v>0.715333333333333</v>
+      </c>
+      <c r="M26" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="F27" s="2" t="n">
         <f aca="false">40/60</f>
@@ -961,16 +1525,39 @@
         <f aca="false">75/100</f>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H27" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <f aca="false">40/50</f>
+        <v>0.8</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <f aca="false">0.2*F27+0.2*G27+0.2*H27+0.2*I27+0.2*J27</f>
+        <v>0.843333333333333</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <f aca="false">K27+0.03</f>
+        <v>0.873333333333333</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F28" s="1" t="n">
         <f aca="false">53/60</f>
@@ -984,7 +1571,27 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
-    </row>
+      <c r="I28" s="0" t="n">
+        <f aca="false">47/50</f>
+        <v>0.94</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <f aca="false">0.2*F28+0.2*G28+0.2*H28+0.2*I28+0.2*J28</f>
+        <v>0.954666666666667</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <f aca="false">K28+0.03</f>
+        <v>0.984666666666667</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>